<commit_message>
update algo to day of year
</commit_message>
<xml_diff>
--- a/effectivecopy.xlsx
+++ b/effectivecopy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repor\autoWPpost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repor\azure\autoWP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E672A32E-D8B6-4DEC-9F53-71482008B004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98875025-6B49-4B76-ABCA-764B71A94945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12225" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{4E0E7364-A766-4D47-91FA-F2E24CD592D9}"/>
   </bookViews>
@@ -1607,8 +1607,8 @@
   <dimension ref="A1:A999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="1" topLeftCell="A291" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E305" sqref="E305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>